<commit_message>
inicio do desenvolvimento do relatório
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://novasbe365-my.sharepoint.com/personal/joao_correia_novasbe_pt/Documents/Documentos/AoL2324/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="92" documentId="8_{149CCACC-2926-4A9B-A287-B32B347C5AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C72A682-6B47-44A0-A86B-A158CA55D982}"/>
+  <xr:revisionPtr revIDLastSave="97" documentId="8_{149CCACC-2926-4A9B-A287-B32B347C5AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8EDF3F50-471A-4922-BAE7-5ADC0BC7D4FC}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="7" xr2:uid="{D81DDF1A-8F59-4540-80B3-E625B03C8271}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="5" xr2:uid="{D81DDF1A-8F59-4540-80B3-E625B03C8271}"/>
   </bookViews>
   <sheets>
     <sheet name="Values and Objectives" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,12 @@
     <sheet name="Courses and Outcomes" sheetId="3" r:id="rId3"/>
     <sheet name="Outcomes and Programs" sheetId="4" r:id="rId4"/>
     <sheet name="Proficiency" sheetId="5" r:id="rId5"/>
-    <sheet name="Program list" sheetId="6" r:id="rId6"/>
-    <sheet name="Configuração" sheetId="7" r:id="rId7"/>
+    <sheet name="Configuração" sheetId="7" r:id="rId6"/>
+    <sheet name="Program list" sheetId="6" r:id="rId7"/>
     <sheet name="Courses" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Configuração!$A$1:$H$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Configuração!$A$1:$H$35</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Courses and Outcomes'!$A$1:$J$134</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3454" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3452" uniqueCount="338">
   <si>
     <t>Course</t>
   </si>
@@ -961,9 +961,6 @@
   </si>
   <si>
     <t>Developing Economics II</t>
-  </si>
-  <si>
-    <t>Cadeira</t>
   </si>
   <si>
     <t>Pinciples of Macroeconomics</t>
@@ -16081,6 +16078,943 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E63FD22D-8CB2-4CF1-8FD0-6C265F057293}">
+  <dimension ref="A1:H35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:H35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.08984375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="5.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.7265625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2324</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="7">
+        <v>1118</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2324</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" s="7">
+        <v>1310</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2324</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" s="7">
+        <v>1313</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2324</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="7">
+        <v>1124</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2324</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="7">
+        <v>1462</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2324</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="7">
+        <v>1312</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2324</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="E8" s="7">
+        <v>1463</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2324</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="7">
+        <v>1218</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1">
+        <v>2324</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="7">
+        <v>1310</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1">
+        <v>2324</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="7">
+        <v>1313</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2324</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" s="7">
+        <v>1312</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>15</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2324</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="7">
+        <v>2414</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>15</v>
+      </c>
+      <c r="B14" s="1">
+        <v>2324</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" s="7">
+        <v>2584</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>15</v>
+      </c>
+      <c r="B15" s="1">
+        <v>2324</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="7">
+        <v>2336</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1">
+        <v>2324</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" s="7">
+        <v>2168</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>14</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2324</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" s="7">
+        <v>2188</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1">
+        <v>2324</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="7">
+        <v>2270</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>37</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2324</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" s="7">
+        <v>2346</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>37</v>
+      </c>
+      <c r="B20" s="1">
+        <v>2324</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" s="7">
+        <v>2607</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>38</v>
+      </c>
+      <c r="B21" s="1">
+        <v>2324</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E21" s="7">
+        <v>2628</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>38</v>
+      </c>
+      <c r="B22" s="1">
+        <v>2324</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E22" s="7">
+        <v>2710</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>39</v>
+      </c>
+      <c r="B23" s="1">
+        <v>2324</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E23" s="7">
+        <v>2746</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>39</v>
+      </c>
+      <c r="B24" s="1">
+        <v>2324</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" s="7">
+        <v>2739</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>39</v>
+      </c>
+      <c r="B25" s="1">
+        <v>2324</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" s="7">
+        <v>2742</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>27</v>
+      </c>
+      <c r="B26" s="1">
+        <v>2324</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E26" s="7">
+        <v>6101</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>27</v>
+      </c>
+      <c r="B27" s="1">
+        <v>2324</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E27" s="7">
+        <v>6124</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1">
+        <v>2324</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E28" s="7">
+        <v>6109</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>33</v>
+      </c>
+      <c r="B29" s="1">
+        <v>2324</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E29" s="7">
+        <v>6202</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>33</v>
+      </c>
+      <c r="B30" s="1">
+        <v>2324</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E30" s="7">
+        <v>6214</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>37</v>
+      </c>
+      <c r="B31" s="1">
+        <v>2324</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E31" s="7">
+        <v>2597</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>16</v>
+      </c>
+      <c r="B32" s="1">
+        <v>2324</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E32" s="7">
+        <v>2269</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>15</v>
+      </c>
+      <c r="B33" s="1">
+        <v>2324</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E33" s="7">
+        <v>2581</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>2</v>
+      </c>
+      <c r="B34" s="1">
+        <v>2324</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E34" s="7">
+        <v>1462</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>27</v>
+      </c>
+      <c r="B35" s="1">
+        <v>2324</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E35" s="7">
+        <v>6121</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:H35" xr:uid="{E63FD22D-8CB2-4CF1-8FD0-6C265F057293}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1AF9503-9B6B-4A72-802D-E5FA653468E2}">
   <dimension ref="A1:B13"/>
   <sheetViews>
@@ -16205,949 +17139,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E63FD22D-8CB2-4CF1-8FD0-6C265F057293}">
-  <dimension ref="A1:H35"/>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6427C803-0B28-4EA1-8230-C6C35778DEE6}">
+  <dimension ref="A1:B88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S35" sqref="S35"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="6.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.08984375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="5.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="6"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>2324</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E2" s="7">
-        <v>1118</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1">
-        <v>2324</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E3" s="7">
-        <v>1310</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1">
-        <v>2324</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E4" s="7">
-        <v>1313</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1">
-        <v>2324</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E5" s="7">
-        <v>1124</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>1</v>
-      </c>
-      <c r="B6" s="1">
-        <v>2324</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E6" s="7">
-        <v>1462</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>1</v>
-      </c>
-      <c r="B7" s="1">
-        <v>2324</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E7" s="7">
-        <v>1312</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>1</v>
-      </c>
-      <c r="B8" s="1">
-        <v>2324</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="E8" s="7">
-        <v>1463</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>2</v>
-      </c>
-      <c r="B9" s="1">
-        <v>2324</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E9" s="7">
-        <v>1218</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
-        <v>2</v>
-      </c>
-      <c r="B10" s="1">
-        <v>2324</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E10" s="7">
-        <v>1310</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <v>2</v>
-      </c>
-      <c r="B11" s="1">
-        <v>2324</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E11" s="7">
-        <v>1313</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
-        <v>2</v>
-      </c>
-      <c r="B12" s="1">
-        <v>2324</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E12" s="7">
-        <v>1312</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
-        <v>15</v>
-      </c>
-      <c r="B13" s="1">
-        <v>2324</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E13" s="7">
-        <v>2414</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
-        <v>15</v>
-      </c>
-      <c r="B14" s="1">
-        <v>2324</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E14" s="7">
-        <v>2584</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
-        <v>15</v>
-      </c>
-      <c r="B15" s="1">
-        <v>2324</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E15" s="7">
-        <v>2336</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
-        <v>14</v>
-      </c>
-      <c r="B16" s="1">
-        <v>2324</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E16" s="7">
-        <v>2168</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
-        <v>14</v>
-      </c>
-      <c r="B17" s="1">
-        <v>2324</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E17" s="7">
-        <v>2188</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
-        <v>16</v>
-      </c>
-      <c r="B18" s="1">
-        <v>2324</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E18" s="7">
-        <v>2270</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
-        <v>37</v>
-      </c>
-      <c r="B19" s="1">
-        <v>2324</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E19" s="7">
-        <v>2346</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
-        <v>37</v>
-      </c>
-      <c r="B20" s="1">
-        <v>2324</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E20" s="7">
-        <v>2607</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
-        <v>38</v>
-      </c>
-      <c r="B21" s="1">
-        <v>2324</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E21" s="7">
-        <v>2628</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="H21" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
-        <v>38</v>
-      </c>
-      <c r="B22" s="1">
-        <v>2324</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E22" s="7">
-        <v>2710</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="H22" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
-        <v>39</v>
-      </c>
-      <c r="B23" s="1">
-        <v>2324</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E23" s="7">
-        <v>2746</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="H23" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
-        <v>39</v>
-      </c>
-      <c r="B24" s="1">
-        <v>2324</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E24" s="7">
-        <v>2739</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="H24" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="1">
-        <v>39</v>
-      </c>
-      <c r="B25" s="1">
-        <v>2324</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E25" s="7">
-        <v>2742</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="H25" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="1">
-        <v>27</v>
-      </c>
-      <c r="B26" s="1">
-        <v>2324</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E26" s="7">
-        <v>6101</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="H26" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="1">
-        <v>27</v>
-      </c>
-      <c r="B27" s="1">
-        <v>2324</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E27" s="7">
-        <v>6124</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="1">
-        <v>27</v>
-      </c>
-      <c r="B28" s="1">
-        <v>2324</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E28" s="7">
-        <v>6109</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="H28" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="1">
-        <v>33</v>
-      </c>
-      <c r="B29" s="1">
-        <v>2324</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E29" s="7">
-        <v>6202</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="H29" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="1">
-        <v>33</v>
-      </c>
-      <c r="B30" s="1">
-        <v>2324</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E30" s="7">
-        <v>6214</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="H30" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="1">
-        <v>37</v>
-      </c>
-      <c r="B31" s="1">
-        <v>2324</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E31" s="7">
-        <v>2597</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="H31" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="1">
-        <v>16</v>
-      </c>
-      <c r="B32" s="1">
-        <v>2324</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E32" s="7">
-        <v>2269</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="H32" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="1">
-        <v>15</v>
-      </c>
-      <c r="B33" s="1">
-        <v>2324</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E33" s="7">
-        <v>2581</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="H33" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="1">
-        <v>2</v>
-      </c>
-      <c r="B34" s="1">
-        <v>2324</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E34" s="7">
-        <v>1462</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="H34" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="1">
-        <v>27</v>
-      </c>
-      <c r="B35" s="1">
-        <v>2324</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E35" s="7">
-        <v>6121</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="H35" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:H35" xr:uid="{E63FD22D-8CB2-4CF1-8FD0-6C265F057293}"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6427C803-0B28-4EA1-8230-C6C35778DEE6}">
-  <dimension ref="A1:B89"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B36"/>
+      <selection sqref="A1:B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.3"/>
@@ -17166,8 +17163,8 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>271</v>
+      <c r="A2" s="1">
+        <v>1118</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>305</v>
@@ -17175,31 +17172,31 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>1118</v>
+        <v>1310</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>306</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>1310</v>
+        <v>1313</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>1313</v>
+        <v>1124</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>103</v>
+        <v>306</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>1124</v>
+        <v>1462</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>307</v>
@@ -17207,87 +17204,87 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>1462</v>
+        <v>1312</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>308</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>1312</v>
+        <v>1463</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>102</v>
+        <v>308</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>1463</v>
+        <v>1218</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>309</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>1218</v>
+        <v>1310</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>1310</v>
+        <v>1313</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>1312</v>
+        <v>2414</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>2414</v>
+        <v>2584</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
-        <v>2584</v>
+        <v>2336</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
-        <v>2336</v>
+        <v>2168</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>119</v>
+        <v>309</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
-        <v>2168</v>
+        <v>2188</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>310</v>
@@ -17295,39 +17292,39 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
-        <v>2188</v>
+        <v>2270</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>311</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>2270</v>
+        <v>2346</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <v>2346</v>
+        <v>2607</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
-        <v>2607</v>
+        <v>2628</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>154</v>
+        <v>311</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
-        <v>2628</v>
+        <v>2710</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>312</v>
@@ -17335,39 +17332,39 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
-        <v>2710</v>
+        <v>2746</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>313</v>
+        <v>160</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
-        <v>2746</v>
+        <v>2739</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
-        <v>2739</v>
+        <v>2742</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
-        <v>2742</v>
+        <v>6101</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>158</v>
+        <v>313</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
-        <v>6101</v>
+        <v>6124</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>314</v>
@@ -17375,7 +17372,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
-        <v>6124</v>
+        <v>6109</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>315</v>
@@ -17383,67 +17380,63 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
-        <v>6109</v>
+        <v>6202</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>316</v>
+        <v>172</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
-        <v>6202</v>
+        <v>6214</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
-        <v>6214</v>
+        <v>2597</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>177</v>
+        <v>152</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
-        <v>2597</v>
+        <v>2269</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>152</v>
+        <v>316</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
-        <v>2269</v>
+        <v>2581</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>317</v>
+        <v>131</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
-        <v>2581</v>
+        <v>1462</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>131</v>
+        <v>307</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
-        <v>1462</v>
+        <v>6121</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="1">
-        <v>6121</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>318</v>
-      </c>
+        <v>317</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A58"/>
+      <c r="B58"/>
     </row>
     <row r="59" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A59"/>
@@ -17451,10 +17444,10 @@
     </row>
     <row r="60" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A60"/>
-      <c r="B60"/>
     </row>
     <row r="61" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A61"/>
+      <c r="B61"/>
     </row>
     <row r="62" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A62"/>
@@ -17563,10 +17556,6 @@
     <row r="88" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A88"/>
       <c r="B88"/>
-    </row>
-    <row r="89" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A89"/>
-      <c r="B89"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>